<commit_message>
finish bildings, add spy_fact_temp
</commit_message>
<xml_diff>
--- a/bilds.xlsx
+++ b/bilds.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFA51C9-9B14-4079-9361-C179AD086348}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -88,10 +87,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -136,7 +135,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -145,7 +144,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
@@ -428,16 +427,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -469,7 +468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -481,7 +480,7 @@
         <v>3.1740000000000004</v>
       </c>
       <c r="D2" s="1">
-        <v>23339</v>
+        <v>31914</v>
       </c>
       <c r="E2" s="1">
         <v>1.3</v>
@@ -496,7 +495,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -508,7 +507,7 @@
         <v>3.1740000000000004</v>
       </c>
       <c r="D3" s="1">
-        <v>23940.000000000004</v>
+        <v>36167</v>
       </c>
       <c r="E3" s="1">
         <v>1.3</v>
@@ -523,7 +522,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -535,7 +534,7 @@
         <v>3.6</v>
       </c>
       <c r="D4" s="1">
-        <v>35524</v>
+        <v>45221</v>
       </c>
       <c r="E4" s="1">
         <v>1.85</v>
@@ -550,7 +549,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -562,7 +561,7 @@
         <v>3.6766666666666672</v>
       </c>
       <c r="D5" s="1">
-        <v>20643</v>
+        <v>32960</v>
       </c>
       <c r="E5" s="1">
         <v>1.3</v>
@@ -577,7 +576,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -589,7 +588,7 @@
         <v>4.339999999999999</v>
       </c>
       <c r="D6" s="1">
-        <v>93367.550399999993</v>
+        <v>118910</v>
       </c>
       <c r="E6" s="1">
         <v>1.3</v>
@@ -604,7 +603,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -616,7 +615,7 @@
         <v>8.75</v>
       </c>
       <c r="D7" s="1">
-        <v>14940</v>
+        <v>86979</v>
       </c>
       <c r="E7" s="1">
         <v>1.3</v>
@@ -631,7 +630,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -643,7 +642,7 @@
         <v>3.8066666666666666</v>
       </c>
       <c r="D8" s="1">
-        <v>91641.600000000006</v>
+        <v>17105</v>
       </c>
       <c r="E8" s="1">
         <v>1.3</v>
@@ -658,7 +657,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -670,7 +669,7 @@
         <v>20.471428571428572</v>
       </c>
       <c r="D9" s="1">
-        <v>524888.5416</v>
+        <v>517516</v>
       </c>
       <c r="E9" s="1">
         <v>1.3</v>
@@ -685,7 +684,7 @@
       <c r="I9" s="2"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -697,7 +696,7 @@
         <v>23</v>
       </c>
       <c r="D10" s="1">
-        <v>475105.19999999995</v>
+        <v>469399</v>
       </c>
       <c r="E10" s="1">
         <v>1.3</v>

</xml_diff>

<commit_message>
update bilds and fact heat
</commit_message>
<xml_diff>
--- a/bilds.xlsx
+++ b/bilds.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801B1352-DC10-4D0E-815F-13BB0690937A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14091" windowHeight="5229" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,41 +58,41 @@
     <t>manufactory</t>
   </si>
   <si>
-    <t>SABZ</t>
-  </si>
-  <si>
-    <t>UABZ</t>
-  </si>
-  <si>
-    <t>ZY</t>
-  </si>
-  <si>
-    <t>CZL</t>
-  </si>
-  <si>
-    <t>IK</t>
-  </si>
-  <si>
-    <t>m_24</t>
-  </si>
-  <si>
-    <t>abz_24</t>
-  </si>
-  <si>
-    <t>m_202</t>
-  </si>
-  <si>
-    <t>m_28</t>
+    <t>ЮАБЗ</t>
+  </si>
+  <si>
+    <t>САБЗ</t>
+  </si>
+  <si>
+    <t>ЗУ</t>
+  </si>
+  <si>
+    <t>ЦЗЛ</t>
+  </si>
+  <si>
+    <t>Инженерный корпус</t>
+  </si>
+  <si>
+    <t>24 цех</t>
+  </si>
+  <si>
+    <t>28 цех</t>
+  </si>
+  <si>
+    <t>202 цех</t>
+  </si>
+  <si>
+    <t>24 цех АБЗ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -135,7 +136,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -144,8 +145,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -427,16 +428,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -468,9 +469,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -495,9 +496,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -522,7 +523,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -549,7 +550,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -576,7 +577,7 @@
       <c r="I5" s="2"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -603,7 +604,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -630,9 +631,9 @@
       <c r="I7" s="2"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -657,7 +658,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -684,9 +685,9 @@
       <c r="I9" s="2"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>

</xml_diff>